<commit_message>
V0.7.1 Improved Excel layout
Turned the headers of the columns 90 degrees so it is easier to read the headers when filling the sheet.
</commit_message>
<xml_diff>
--- a/dws_squid.xlsx
+++ b/dws_squid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Development\anDREa_squid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5F060D-B0F0-4031-A136-C82C3AFAA4BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D97955A-9550-4C4F-82DD-4173CBCDC721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4470" yWindow="3225" windowWidth="28800" windowHeight="15435" xr2:uid="{EB91D85B-3B10-4E01-B68C-94971D77060D}"/>
   </bookViews>
@@ -117,14 +117,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="180" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -440,36 +444,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CA32C8D-AEDA-4870-A630-41EECB6AF2B4}">
-  <dimension ref="A1:FM5"/>
+  <dimension ref="A1:FM10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2" max="169" width="9.140625" style="2"/>
+    <col min="2" max="63" width="4.42578125" style="3" customWidth="1"/>
+    <col min="64" max="169" width="9.140625" style="3"/>
     <col min="170" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" s="5" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -477,10 +482,10 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -493,13 +498,13 @@
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -507,9 +512,12 @@
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="3" t="s">
         <v>6</v>
       </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
V0.7.2 Removed the need to have '.' in front of domain in Excel
The '.' will be programmatically added.  Easier for people to just fill in the domain name.
</commit_message>
<xml_diff>
--- a/dws_squid.xlsx
+++ b/dws_squid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Development\anDREa_squid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D97955A-9550-4C4F-82DD-4173CBCDC721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBEDB82-47F7-4FD1-811E-82B6EE92DBC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4470" yWindow="3225" windowWidth="28800" windowHeight="15435" xr2:uid="{EB91D85B-3B10-4E01-B68C-94971D77060D}"/>
   </bookViews>
@@ -40,12 +40,6 @@
     <t>WorkspaceID</t>
   </si>
   <si>
-    <t>.google.com</t>
-  </si>
-  <si>
-    <t>.nu.nl</t>
-  </si>
-  <si>
     <t>dws001test001</t>
   </si>
   <si>
@@ -58,16 +52,22 @@
     <t>x</t>
   </si>
   <si>
-    <t>.tweaker.net</t>
-  </si>
-  <si>
-    <t>.bbc.com</t>
-  </si>
-  <si>
     <t>dws004test004</t>
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>google.com</t>
+  </si>
+  <si>
+    <t>nu.nl</t>
+  </si>
+  <si>
+    <t>tweaker.net</t>
+  </si>
+  <si>
+    <t>bbc.com</t>
   </si>
 </sst>
 </file>
@@ -450,7 +450,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,54 +466,54 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="D4" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
V0.8 Basic domain validation
Domains that do not match requirements of a normal URL will be skipped and listed in a WRONG_DOMAINS.txt
</commit_message>
<xml_diff>
--- a/dws_squid.xlsx
+++ b/dws_squid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Development\anDREa_squid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8FF33FB-0DAE-4643-AACE-6E5A8FDE5722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE8FACF-8657-4A98-9259-11501E1A1EDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4470" yWindow="3225" windowWidth="28800" windowHeight="15435" xr2:uid="{EB91D85B-3B10-4E01-B68C-94971D77060D}"/>
+    <workbookView xWindow="6135" yWindow="3225" windowWidth="28800" windowHeight="15435" xr2:uid="{EB91D85B-3B10-4E01-B68C-94971D77060D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
   <si>
     <t>WorkspaceID</t>
   </si>
@@ -71,13 +71,31 @@
   </si>
   <si>
     <t>dws004test005</t>
+  </si>
+  <si>
+    <t>github.com</t>
+  </si>
+  <si>
+    <t>.wrong.url</t>
+  </si>
+  <si>
+    <t>www.test.com</t>
+  </si>
+  <si>
+    <t>bbc.com/subsite</t>
+  </si>
+  <si>
+    <t>https://wwww.google.com</t>
+  </si>
+  <si>
+    <t>https://google.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +113,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -117,10 +143,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -133,8 +160,12 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="180" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="180" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -449,11 +480,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CA32C8D-AEDA-4870-A630-41EECB6AF2B4}">
   <dimension ref="A1:FM10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,7 +495,7 @@
     <col min="170" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="5" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="5" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -480,8 +511,26 @@
       <c r="E1" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="F1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -491,13 +540,31 @@
       <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -511,28 +578,45 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="F5" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="G6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="H1" r:id="rId1" xr:uid="{AD880A28-C4C8-48FC-9585-F5A45E28E3E5}"/>
+    <hyperlink ref="J1" r:id="rId2" xr:uid="{98FCB6ED-CCFA-41F5-8BF4-154FA2F8665B}"/>
+    <hyperlink ref="K1" r:id="rId3" xr:uid="{564EFEBE-2859-4B4F-AE83-7D3F82F116E1}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
V0.8.1 more test cases
</commit_message>
<xml_diff>
--- a/dws_squid.xlsx
+++ b/dws_squid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Development\anDREa_squid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE8FACF-8657-4A98-9259-11501E1A1EDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F86D57A-A3B6-459A-B288-1B48E486D0E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6135" yWindow="3225" windowWidth="28800" windowHeight="15435" xr2:uid="{EB91D85B-3B10-4E01-B68C-94971D77060D}"/>
+    <workbookView xWindow="2475" yWindow="6915" windowWidth="28800" windowHeight="15435" xr2:uid="{EB91D85B-3B10-4E01-B68C-94971D77060D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="22">
   <si>
     <t>WorkspaceID</t>
   </si>
@@ -89,6 +89,18 @@
   </si>
   <si>
     <t>https://google.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> google.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">google.com </t>
+  </si>
+  <si>
+    <t>google .com</t>
+  </si>
+  <si>
+    <t>google. Com</t>
   </si>
 </sst>
 </file>
@@ -484,7 +496,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K4" sqref="K4"/>
+      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,7 +507,7 @@
     <col min="170" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="5" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="5" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -529,8 +541,20 @@
       <c r="K1" s="6" t="s">
         <v>17</v>
       </c>
+      <c r="L1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -558,13 +582,25 @@
       <c r="K2" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="L2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -578,7 +614,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -589,7 +625,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -606,7 +642,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
V0.8.3 Excel Col ID is now correct after Z.
</commit_message>
<xml_diff>
--- a/dws_squid.xlsx
+++ b/dws_squid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Development\anDREa_squid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F86D57A-A3B6-459A-B288-1B48E486D0E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1182631-D109-4DD1-8C9F-8EEC0CBB7D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2475" yWindow="6915" windowWidth="28800" windowHeight="15435" xr2:uid="{EB91D85B-3B10-4E01-B68C-94971D77060D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="23">
   <si>
     <t>WorkspaceID</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>google. Com</t>
+  </si>
+  <si>
+    <t>sub.google.com</t>
   </si>
 </sst>
 </file>
@@ -493,10 +496,10 @@
   <dimension ref="A1:FM10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="BR2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
+      <selection pane="bottomRight" activeCell="P1" sqref="P1:BS2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,7 +510,7 @@
     <col min="170" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="5" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:71" s="5" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -553,8 +556,176 @@
       <c r="O1" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="P1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AH1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AI1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AJ1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AK1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AL1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AM1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AN1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AO1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AP1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AQ1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AR1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AS1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AT1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AU1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AW1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AX1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AY1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AZ1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="BA1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="BB1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="BC1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="BD1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="BE1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="BF1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="BG1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="BH1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="BI1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="BJ1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="BK1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="BL1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="BM1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="BN1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="BO1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="BP1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="BQ1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="BR1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="BS1" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -594,13 +765,181 @@
       <c r="O2" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="P2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AL2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AM2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AN2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AO2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AP2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AQ2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AR2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AS2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AT2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AU2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AV2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AW2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AX2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AY2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AZ2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BA2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BC2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BD2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BE2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BF2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BG2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BH2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BI2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BJ2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BK2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BM2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BN2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BO2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BP2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BQ2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BR2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BS2" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -614,7 +953,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -625,7 +964,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -642,7 +981,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
V0.9 Move all variables to an .ini file
Remove all variables to an .ini file.  The name of the .ini file must match the filename of the python script with the .py extension replaced with .ini  (default: workspace_whitelist.ini)
</commit_message>
<xml_diff>
--- a/dws_squid.xlsx
+++ b/dws_squid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Development\anDREa_squid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71AF87BD-8B7E-4F1A-BA1A-EBA5209C351D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F217B00-90A8-4CB6-B521-A6E92A4B9320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2475" yWindow="6915" windowWidth="28800" windowHeight="15435" xr2:uid="{EB91D85B-3B10-4E01-B68C-94971D77060D}"/>
+    <workbookView xWindow="2100" yWindow="3105" windowWidth="28800" windowHeight="15435" xr2:uid="{EB91D85B-3B10-4E01-B68C-94971D77060D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="24">
   <si>
     <t>WorkspaceID</t>
   </si>
@@ -499,10 +499,10 @@
   <dimension ref="A1:FM10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="BS2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P2" sqref="P2"/>
+      <selection pane="bottomRight" activeCell="BY3" sqref="BY3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,7 +513,7 @@
     <col min="170" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:71" s="5" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:81" s="5" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -727,8 +727,38 @@
       <c r="BS1" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="BT1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="BU1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="BV1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="BW1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="BX1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="BY1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="BZ1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="CA1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="CB1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="CC1" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -936,13 +966,43 @@
       <c r="BS2" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="BT2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BU2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BV2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BW2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BX2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BY2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BZ2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="CA2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="CB2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="CC2" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -956,7 +1016,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -967,7 +1027,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -984,7 +1044,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
     </row>
   </sheetData>

</xml_diff>